<commit_message>
fix GL Payable detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_payable.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_payable.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t xml:space="preserve">GL Payable Report</t>
   </si>
   <si>
+    <t xml:space="preserve">Account Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partner</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fiscal Year From</t>
   </si>
   <si>
@@ -53,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">Charge Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Code</t>
   </si>
   <si>
     <t xml:space="preserve">Account Name</t>
@@ -206,9 +209,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -233,13 +235,13 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="arial"/>
       <family val="2"/>
@@ -262,7 +264,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFADC5E7"/>
+        <fgColor rgb="FFCCCCFF"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
@@ -313,14 +315,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,16 +342,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,66 +363,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FFADC5E7"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -429,26 +371,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX10"/>
+  <dimension ref="A1:AX12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="51" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -459,202 +447,214 @@
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="J12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="K12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="M12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="N12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="O12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="P12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="10" t="s">
+      <c r="Q12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="S10" s="10" t="s">
+      <c r="R12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="T10" s="10" t="s">
+      <c r="S12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="T12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="V10" s="10" t="s">
+      <c r="U12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="W10" s="10" t="s">
+      <c r="V12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="X10" s="10" t="s">
+      <c r="W12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="Y10" s="10" t="s">
+      <c r="X12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="Z10" s="10" t="s">
+      <c r="Y12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AA10" s="10" t="s">
+      <c r="Z12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AB10" s="10" t="s">
+      <c r="AA12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="10" t="s">
+      <c r="AB12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AD10" s="10" t="s">
+      <c r="AC12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AE10" s="10" t="s">
+      <c r="AD12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AF10" s="10" t="s">
+      <c r="AE12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AG10" s="10" t="s">
+      <c r="AF12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AH10" s="10" t="s">
+      <c r="AG12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AI10" s="10" t="s">
+      <c r="AH12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AJ10" s="10" t="s">
+      <c r="AI12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AK10" s="10" t="s">
+      <c r="AJ12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AL10" s="10" t="s">
+      <c r="AK12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="AM10" s="10" t="s">
+      <c r="AL12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AN10" s="10" t="s">
+      <c r="AM12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AO10" s="10" t="s">
+      <c r="AN12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AP10" s="10" t="s">
+      <c r="AO12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AQ10" s="10" t="s">
+      <c r="AP12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AR10" s="10" t="s">
+      <c r="AQ12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AS10" s="10" t="s">
+      <c r="AR12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AT10" s="10" t="s">
+      <c r="AS12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AU10" s="10" t="s">
+      <c r="AT12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AV10" s="10" t="s">
+      <c r="AU12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AW10" s="10" t="s">
+      <c r="AV12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AX10" s="10" t="s">
+      <c r="AW12" s="9" t="s">
         <v>59</v>
+      </c>
+      <c r="AX12" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>